<commit_message>
Issues with multiple rows were solved.
</commit_message>
<xml_diff>
--- a/Base.xlsx
+++ b/Base.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCsito\Desktop\CvLAC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UAPA Equipo 02\Desktop\Cvlac\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,6 @@
     <definedName name="Nombre">#REF!</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Departamento de Ingeniería de Sistemas e Industrial</t>
   </si>
@@ -57,6 +56,51 @@
   </si>
   <si>
     <t>Octavio José</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>Adarme Jaimes</t>
+  </si>
+  <si>
+    <t>Jairo Hernán</t>
+  </si>
+  <si>
+    <t>Aponte Melo</t>
+  </si>
+  <si>
+    <t>Emiliano</t>
+  </si>
+  <si>
+    <t>Barreto Hernández</t>
+  </si>
+  <si>
+    <t>Libia Denise</t>
+  </si>
+  <si>
+    <t>Cangrejo Aljure</t>
+  </si>
+  <si>
+    <t>Ismael</t>
+  </si>
+  <si>
+    <t>Castañeda Fuentes</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000439185</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001333865</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001370358</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000199087</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000025410</t>
   </si>
 </sst>
 </file>
@@ -147,7 +191,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -157,6 +201,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -501,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B34B1D23-DD65-40B1-A4A6-4F31B4D45939}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,10 +595,96 @@
         <v>7</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>123123123</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>123123123</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>123123123</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>123123123</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>123123123</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>22</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{DF7EAEED-8BD3-4208-9F09-BBA96ABEA1D9}"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{000B695E-C661-4936-B93F-4874A4D331A3}"/>
+    <hyperlink ref="E5" r:id="rId2" xr:uid="{259D0730-0758-43F1-9290-E0FB73C810B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Little correction on eventos.py.
</commit_message>
<xml_diff>
--- a/Base.xlsx
+++ b/Base.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\UAPA Equipo 02\Desktop\Cvlac\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCsito\Desktop\Cvlac\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="96">
   <si>
     <t>Departamento de Ingeniería de Sistemas e Industrial</t>
   </si>
@@ -101,6 +101,222 @@
   </si>
   <si>
     <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000025410</t>
+  </si>
+  <si>
+    <t>Christian Johannes</t>
+  </si>
+  <si>
+    <t>Bruszies</t>
+  </si>
+  <si>
+    <t>Jean Pierre</t>
+  </si>
+  <si>
+    <t>Charalambos Hernández</t>
+  </si>
+  <si>
+    <t>Javier Francisco</t>
+  </si>
+  <si>
+    <t>López Parra</t>
+  </si>
+  <si>
+    <t>Gabriel José</t>
+  </si>
+  <si>
+    <t>Mañana Guichon</t>
+  </si>
+  <si>
+    <t>Jorge Eduardo</t>
+  </si>
+  <si>
+    <t>Ortiz Triviño</t>
+  </si>
+  <si>
+    <t>Ingrid Patricia</t>
+  </si>
+  <si>
+    <t>Páez Parra</t>
+  </si>
+  <si>
+    <t>Cesar Augusto</t>
+  </si>
+  <si>
+    <t>Pedraza Bonilla</t>
+  </si>
+  <si>
+    <t>Felipe</t>
+  </si>
+  <si>
+    <t>Restrepo Calle</t>
+  </si>
+  <si>
+    <t>Sandra Liliana</t>
+  </si>
+  <si>
+    <t>Rojas Martínez</t>
+  </si>
+  <si>
+    <t>Juan Carlos</t>
+  </si>
+  <si>
+    <t>Torres Pardo</t>
+  </si>
+  <si>
+    <t>Edgar Miguel</t>
+  </si>
+  <si>
+    <t>Vargas Chaparro</t>
+  </si>
+  <si>
+    <t>Jorge Eliecer</t>
+  </si>
+  <si>
+    <t>Camargo Mendoza</t>
+  </si>
+  <si>
+    <t>Oscar Fernando</t>
+  </si>
+  <si>
+    <t>Castellanos Domínguez</t>
+  </si>
+  <si>
+    <t>Félix Antonio</t>
+  </si>
+  <si>
+    <t>Cortes Aldana</t>
+  </si>
+  <si>
+    <t>Helga</t>
+  </si>
+  <si>
+    <t>Duarte Amaya</t>
+  </si>
+  <si>
+    <t>Jonatan</t>
+  </si>
+  <si>
+    <t>Gómez Perdomo</t>
+  </si>
+  <si>
+    <t>Fabio Augusto</t>
+  </si>
+  <si>
+    <t>González Osorio</t>
+  </si>
+  <si>
+    <t>German Jairo</t>
+  </si>
+  <si>
+    <t>Hernández Pérez</t>
+  </si>
+  <si>
+    <t>Elizabeth</t>
+  </si>
+  <si>
+    <t>León Guzmán</t>
+  </si>
+  <si>
+    <t>Sonia Esperanza</t>
+  </si>
+  <si>
+    <t>Monroy Varela</t>
+  </si>
+  <si>
+    <t>Carlos Eduardo</t>
+  </si>
+  <si>
+    <t>Moreno Mantilla</t>
+  </si>
+  <si>
+    <t>Luis Fernando</t>
+  </si>
+  <si>
+    <t>Niño Vásquez</t>
+  </si>
+  <si>
+    <t>José Ismael</t>
+  </si>
+  <si>
+    <t>Peña Reyes</t>
+  </si>
+  <si>
+    <t>Jenny Marcela</t>
+  </si>
+  <si>
+    <t>Sánchez Torres</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001338568</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000224596</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000293075</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000343854</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000226130</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000338885</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000407984</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000499625</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001050524</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001337037</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000812927</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000486388</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000105260</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0001085468</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000099112</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000463388</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000343838</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000230405</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000672610</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000634557</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000212350</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000343846</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000639508</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000480231</t>
   </si>
 </sst>
 </file>
@@ -546,10 +762,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B34B1D23-DD65-40B1-A4A6-4F31B4D45939}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -580,24 +796,24 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>123123123</v>
+        <v>123</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>7</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
-        <v>123123123</v>
+        <v>123</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
@@ -614,7 +830,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
-        <v>123123123</v>
+        <v>123</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -631,7 +847,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
-        <v>123123123</v>
+        <v>123</v>
       </c>
       <c r="B5" t="s">
         <v>13</v>
@@ -648,7 +864,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
-        <v>123123123</v>
+        <v>123</v>
       </c>
       <c r="B6" t="s">
         <v>15</v>
@@ -665,7 +881,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
-        <v>123123123</v>
+        <v>123</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -678,12 +894,420 @@
       </c>
       <c r="E7" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>123</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E8" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>123</v>
+      </c>
+      <c r="B9" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" t="s">
+        <v>29</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>123</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>123</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>123</v>
+      </c>
+      <c r="B12" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>123</v>
+      </c>
+      <c r="B13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>123</v>
+      </c>
+      <c r="B14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>123</v>
+      </c>
+      <c r="B15" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="3">
+        <v>123</v>
+      </c>
+      <c r="B16" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="3">
+        <v>123</v>
+      </c>
+      <c r="B17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="3">
+        <v>123</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>123</v>
+      </c>
+      <c r="B19" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>123</v>
+      </c>
+      <c r="B20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C20" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>123</v>
+      </c>
+      <c r="B21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C21" t="s">
+        <v>53</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>123</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+      <c r="C22" t="s">
+        <v>55</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>123</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>123</v>
+      </c>
+      <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>59</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E24" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>123</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" t="s">
+        <v>61</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>123</v>
+      </c>
+      <c r="B26" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>123</v>
+      </c>
+      <c r="B27" t="s">
+        <v>64</v>
+      </c>
+      <c r="C27" t="s">
+        <v>65</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>123</v>
+      </c>
+      <c r="B28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C28" t="s">
+        <v>67</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>123</v>
+      </c>
+      <c r="B29" t="s">
+        <v>68</v>
+      </c>
+      <c r="C29" t="s">
+        <v>69</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>123</v>
+      </c>
+      <c r="B30" t="s">
+        <v>8</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>123</v>
+      </c>
+      <c r="B31" t="s">
+        <v>70</v>
+      </c>
+      <c r="C31" t="s">
+        <v>71</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E31" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:E1" xr:uid="{DF7EAEED-8BD3-4208-9F09-BBA96ABEA1D9}"/>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{000B695E-C661-4936-B93F-4874A4D331A3}"/>
+    <hyperlink ref="E2" r:id="rId1" display="http://scienti.colciencias.gov.co:8081/cvlac/visualizador/generarCurriculoCv.do?cod_rh=0000296902" xr:uid="{000B695E-C661-4936-B93F-4874A4D331A3}"/>
     <hyperlink ref="E5" r:id="rId2" xr:uid="{259D0730-0758-43F1-9290-E0FB73C810B2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>